<commit_message>
Recommit without data/cifar-10-python.tar.gz and data/cifar-10-batches-py/*
</commit_message>
<xml_diff>
--- a/outputs/hyperparam_search_mnist_train_grouped_analysis.xlsx
+++ b/outputs/hyperparam_search_mnist_train_grouped_analysis.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-rmadhavan\projects\curvatureStep\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEE8CB0-129D-478C-9EF1-1E521364A6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E92798C-BBF0-4CDA-A726-C37058432F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" activeTab="1" xr2:uid="{923E0CDC-C3D7-421B-8369-4E0352F35392}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" activeTab="2" xr2:uid="{923E0CDC-C3D7-421B-8369-4E0352F35392}"/>
   </bookViews>
   <sheets>
     <sheet name="hyperparam_search_mnist_train_g" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="curvature" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="curvature" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="72">
   <si>
     <t>Optimizer Name</t>
   </si>
@@ -191,6 +192,66 @@
   </si>
   <si>
     <t>ShampooCurvature</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch1</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch10</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch2</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch3</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch4</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch5</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch6</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch7</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch8</t>
+  </si>
+  <si>
+    <t>Mean Training Loss epoch9</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch1</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch10</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch2</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch3</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch4</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch5</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch6</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch7</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch8</t>
+  </si>
+  <si>
+    <t>Std Training Loss epoch9</t>
   </si>
 </sst>
 </file>
@@ -693,7 +754,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -711,6 +772,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1185,7 +1252,7 @@
         <v>3.3633000000000001E-3</v>
       </c>
       <c r="G3" s="1" t="str">
-        <f t="shared" ref="G2:G33" si="1">IF($A3=$A2,"",MIN(C3:C22))</f>
+        <f t="shared" ref="G3:G33" si="1">IF($A3=$A2,"",MIN(C3:C22))</f>
         <v/>
       </c>
       <c r="H3" s="1" t="str">
@@ -13466,7 +13533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E345A74F-CC6F-4DD6-B0B3-DDEB23E95545}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -13781,6 +13848,1068 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD7977E-091C-4FA7-A4E2-2841DE3ED16B}">
+  <dimension ref="A1:U16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="9" customFormat="1" ht="42.75">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.39650999999999997</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.17593</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.13056999999999999</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0.10600999999999999</v>
+      </c>
+      <c r="F2" s="10">
+        <v>9.0359999999999996E-2</v>
+      </c>
+      <c r="G2" s="10">
+        <v>7.8769999999999896E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>6.973E-2</v>
+      </c>
+      <c r="I2" s="10">
+        <v>6.1949999999999901E-2</v>
+      </c>
+      <c r="J2" s="10">
+        <v>5.586E-2</v>
+      </c>
+      <c r="K2" s="10">
+        <v>5.067E-2</v>
+      </c>
+      <c r="L2" s="10">
+        <v>3.5126596444542899E-3</v>
+      </c>
+      <c r="M2" s="10">
+        <v>2.5403630536685999E-3</v>
+      </c>
+      <c r="N2" s="10">
+        <v>2.1401194151521399E-3</v>
+      </c>
+      <c r="O2" s="10">
+        <v>2.1824807495650902E-3</v>
+      </c>
+      <c r="P2" s="10">
+        <v>2.3358082113050199E-3</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>2.0412686686905601E-3</v>
+      </c>
+      <c r="R2" s="10">
+        <v>2.1878706035270402E-3</v>
+      </c>
+      <c r="S2" s="10">
+        <v>1.55008960314485E-3</v>
+      </c>
+      <c r="T2" s="10">
+        <v>1.67544355652797E-3</v>
+      </c>
+      <c r="U2" s="10">
+        <v>2.11715217528956E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.33451999999999998</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.15764</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.12197</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.10183</v>
+      </c>
+      <c r="F3" s="10">
+        <v>8.8569999999999996E-2</v>
+      </c>
+      <c r="G3" s="10">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="H3" s="10">
+        <v>7.0669999999999997E-2</v>
+      </c>
+      <c r="I3" s="10">
+        <v>6.429E-2</v>
+      </c>
+      <c r="J3" s="10">
+        <v>5.8869999999999999E-2</v>
+      </c>
+      <c r="K3" s="10">
+        <v>5.3259999999999898E-2</v>
+      </c>
+      <c r="L3" s="10">
+        <v>7.44622201000092E-3</v>
+      </c>
+      <c r="M3" s="10">
+        <v>4.3025057298690002E-3</v>
+      </c>
+      <c r="N3" s="10">
+        <v>4.4098500856352999E-3</v>
+      </c>
+      <c r="O3" s="10">
+        <v>3.4826713884603001E-3</v>
+      </c>
+      <c r="P3" s="10">
+        <v>4.4251930278049198E-3</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>4.2915938505149499E-3</v>
+      </c>
+      <c r="R3" s="10">
+        <v>3.510001582779E-3</v>
+      </c>
+      <c r="S3" s="10">
+        <v>4.8353903668680101E-3</v>
+      </c>
+      <c r="T3" s="10">
+        <v>4.2557281659220403E-3</v>
+      </c>
+      <c r="U3" s="10">
+        <v>3.9721810409675696E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.33463999999999999</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.12209</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.10172</v>
+      </c>
+      <c r="F4" s="10">
+        <v>8.8459999999999997E-2</v>
+      </c>
+      <c r="G4" s="10">
+        <v>7.9159999999999994E-2</v>
+      </c>
+      <c r="H4" s="10">
+        <v>7.0749999999999993E-2</v>
+      </c>
+      <c r="I4" s="10">
+        <v>6.4070000000000002E-2</v>
+      </c>
+      <c r="J4" s="10">
+        <v>5.8650000000000001E-2</v>
+      </c>
+      <c r="K4" s="10">
+        <v>5.3510000000000002E-2</v>
+      </c>
+      <c r="L4" s="10">
+        <v>7.5997368375490502E-3</v>
+      </c>
+      <c r="M4" s="10">
+        <v>4.9475021756213199E-3</v>
+      </c>
+      <c r="N4" s="10">
+        <v>4.2193864746219003E-3</v>
+      </c>
+      <c r="O4" s="10">
+        <v>3.9608641032537802E-3</v>
+      </c>
+      <c r="P4" s="10">
+        <v>4.3202880562398602E-3</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>4.3484863266811903E-3</v>
+      </c>
+      <c r="R4" s="10">
+        <v>3.9010682297715899E-3</v>
+      </c>
+      <c r="S4" s="10">
+        <v>4.1931293008126199E-3</v>
+      </c>
+      <c r="T4" s="10">
+        <v>4.3856457778631503E-3</v>
+      </c>
+      <c r="U4" s="10">
+        <v>3.6957783723835201E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.38229000000000002</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.19563999999999901</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.14118999999999901</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.11287</v>
+      </c>
+      <c r="F5" s="10">
+        <v>9.4750000000000001E-2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>8.2960000000000006E-2</v>
+      </c>
+      <c r="H5" s="10">
+        <v>7.2669999999999998E-2</v>
+      </c>
+      <c r="I5" s="10">
+        <v>6.5310000000000007E-2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>5.876E-2</v>
+      </c>
+      <c r="K5" s="10">
+        <v>5.4109999999999998E-2</v>
+      </c>
+      <c r="L5" s="10">
+        <v>5.5167321244857601E-3</v>
+      </c>
+      <c r="M5" s="10">
+        <v>5.3145920717293802E-3</v>
+      </c>
+      <c r="N5" s="10">
+        <v>3.9658122329059601E-3</v>
+      </c>
+      <c r="O5" s="10">
+        <v>3.9001566920089498E-3</v>
+      </c>
+      <c r="P5" s="10">
+        <v>3.1570907846025201E-3</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>3.3596296092145502E-3</v>
+      </c>
+      <c r="R5" s="10">
+        <v>3.0074167578763599E-3</v>
+      </c>
+      <c r="S5" s="10">
+        <v>2.7746671472048301E-3</v>
+      </c>
+      <c r="T5" s="10">
+        <v>2.7236413534498598E-3</v>
+      </c>
+      <c r="U5" s="10">
+        <v>2.7646378103148E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.3821</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.19528000000000001</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.14119999999999999</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.113579999999999</v>
+      </c>
+      <c r="F6" s="10">
+        <v>9.6640000000000004E-2</v>
+      </c>
+      <c r="G6" s="10">
+        <v>8.5010000000000002E-2</v>
+      </c>
+      <c r="H6" s="10">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="I6" s="10">
+        <v>6.7879999999999996E-2</v>
+      </c>
+      <c r="J6" s="10">
+        <v>6.2439999999999898E-2</v>
+      </c>
+      <c r="K6" s="10">
+        <v>5.7709999999999997E-2</v>
+      </c>
+      <c r="L6" s="10">
+        <v>5.37359800836976E-3</v>
+      </c>
+      <c r="M6" s="10">
+        <v>5.1744672296876199E-3</v>
+      </c>
+      <c r="N6" s="10">
+        <v>4.2429025704371504E-3</v>
+      </c>
+      <c r="O6" s="10">
+        <v>4.0731642081638002E-3</v>
+      </c>
+      <c r="P6" s="10">
+        <v>2.8087957087216801E-3</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>2.9164095124732401E-3</v>
+      </c>
+      <c r="R6" s="10">
+        <v>2.9024893530286101E-3</v>
+      </c>
+      <c r="S6" s="10">
+        <v>2.77920852042447E-3</v>
+      </c>
+      <c r="T6" s="10">
+        <v>2.88490323350137E-3</v>
+      </c>
+      <c r="U6" s="10">
+        <v>2.33497561253026E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.38242999999999999</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.19519</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.1416</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.11413</v>
+      </c>
+      <c r="F7" s="10">
+        <v>9.7250000000000003E-2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>8.5650000000000004E-2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>7.603E-2</v>
+      </c>
+      <c r="I7" s="10">
+        <v>6.93E-2</v>
+      </c>
+      <c r="J7" s="10">
+        <v>6.3380000000000006E-2</v>
+      </c>
+      <c r="K7" s="10">
+        <v>5.8699999999999898E-2</v>
+      </c>
+      <c r="L7" s="10">
+        <v>5.1781699899138799E-3</v>
+      </c>
+      <c r="M7" s="10">
+        <v>4.9074659675052397E-3</v>
+      </c>
+      <c r="N7" s="10">
+        <v>4.1774527060292497E-3</v>
+      </c>
+      <c r="O7" s="10">
+        <v>3.9539150780516803E-3</v>
+      </c>
+      <c r="P7" s="10">
+        <v>2.78856793195201E-3</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>2.9923049458383802E-3</v>
+      </c>
+      <c r="R7" s="10">
+        <v>2.97995152831569E-3</v>
+      </c>
+      <c r="S7" s="10">
+        <v>2.6599916457679899E-3</v>
+      </c>
+      <c r="T7" s="10">
+        <v>2.8169329262712401E-3</v>
+      </c>
+      <c r="U7" s="10">
+        <v>2.64826987547215E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.37992999999999999</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.17809</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.13930999999999999</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.11817999999999999</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.10502</v>
+      </c>
+      <c r="G8" s="10">
+        <v>9.5449999999999993E-2</v>
+      </c>
+      <c r="H8" s="10">
+        <v>8.745E-2</v>
+      </c>
+      <c r="I8" s="10">
+        <v>8.1070000000000003E-2</v>
+      </c>
+      <c r="J8" s="10">
+        <v>7.4800000000000005E-2</v>
+      </c>
+      <c r="K8" s="10">
+        <v>7.009E-2</v>
+      </c>
+      <c r="L8" s="10">
+        <v>5.7209264983916703E-3</v>
+      </c>
+      <c r="M8" s="10">
+        <v>4.5598367417168601E-3</v>
+      </c>
+      <c r="N8" s="10">
+        <v>4.0137126066634096E-3</v>
+      </c>
+      <c r="O8" s="10">
+        <v>3.35254463886098E-3</v>
+      </c>
+      <c r="P8" s="10">
+        <v>4.5394076950877899E-3</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>4.0349170444453301E-3</v>
+      </c>
+      <c r="R8" s="10">
+        <v>4.6339927588299997E-3</v>
+      </c>
+      <c r="S8" s="10">
+        <v>4.29781598282455E-3</v>
+      </c>
+      <c r="T8" s="10">
+        <v>4.4374667447893102E-3</v>
+      </c>
+      <c r="U8" s="10">
+        <v>3.7397118130204098E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1.5110300000000001</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.38729999999999998</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.28420999999999902</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.23752000000000001</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.20485</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.18046000000000001</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.16148000000000001</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.14627999999999999</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.13371</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.12331</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0.94794292145325498</v>
+      </c>
+      <c r="M9" s="10">
+        <v>2.1348484203281899E-2</v>
+      </c>
+      <c r="N9" s="10">
+        <v>4.1007993800666999E-3</v>
+      </c>
+      <c r="O9" s="10">
+        <v>4.2065557301801003E-3</v>
+      </c>
+      <c r="P9" s="10">
+        <v>4.1371622050762101E-3</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>3.8973495267082899E-3</v>
+      </c>
+      <c r="R9" s="10">
+        <v>3.74842189016478E-3</v>
+      </c>
+      <c r="S9" s="10">
+        <v>3.3976462440931002E-3</v>
+      </c>
+      <c r="T9" s="10">
+        <v>2.9471078101156001E-3</v>
+      </c>
+      <c r="U9" s="10">
+        <v>2.74244416533864E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.34122999999999998</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.16886999999999999</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.13739999999999999</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.12631999999999999</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.12249</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.12197</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0.12092</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.12472999999999999</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.13025</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0.13142999999999999</v>
+      </c>
+      <c r="L10" s="10">
+        <v>4.9772928831287797E-3</v>
+      </c>
+      <c r="M10" s="10">
+        <v>4.3289849977923203E-3</v>
+      </c>
+      <c r="N10" s="10">
+        <v>2.6956755492207598E-3</v>
+      </c>
+      <c r="O10" s="10">
+        <v>2.1462111317906698E-3</v>
+      </c>
+      <c r="P10" s="10">
+        <v>2.1676664360038801E-3</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>2.5144250502517102E-3</v>
+      </c>
+      <c r="R10" s="10">
+        <v>2.76317048173128E-3</v>
+      </c>
+      <c r="S10" s="10">
+        <v>4.2481499241172902E-3</v>
+      </c>
+      <c r="T10" s="10">
+        <v>2.40011573795005E-3</v>
+      </c>
+      <c r="U10" s="10">
+        <v>3.0430430675741499E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0.34081</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.16921</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.13739999999999999</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.12617999999999999</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.12286999999999999</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0.12161</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.12179</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.12503999999999901</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.12858</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.13328000000000001</v>
+      </c>
+      <c r="L11" s="10">
+        <v>4.4955410006904499E-3</v>
+      </c>
+      <c r="M11" s="10">
+        <v>3.9093761934894701E-3</v>
+      </c>
+      <c r="N11" s="10">
+        <v>3.1601687718643499E-3</v>
+      </c>
+      <c r="O11" s="10">
+        <v>2.3999074056212199E-3</v>
+      </c>
+      <c r="P11" s="10">
+        <v>3.0775350887069001E-3</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>2.5937745982769298E-3</v>
+      </c>
+      <c r="R11" s="10">
+        <v>2.4415159225366499E-3</v>
+      </c>
+      <c r="S11" s="10">
+        <v>3.6878780408853501E-3</v>
+      </c>
+      <c r="T11" s="10">
+        <v>2.9954780735116202E-3</v>
+      </c>
+      <c r="U11" s="10">
+        <v>4.9930618528781197E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0.41832000000000003</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.27517000000000003</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.24026</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.21761</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0.20108999999999999</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.18836</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0.17785999999999999</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.16904</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0.16148999999999999</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.15490999999999999</v>
+      </c>
+      <c r="L12" s="10">
+        <v>6.7617880606965098E-3</v>
+      </c>
+      <c r="M12" s="10">
+        <v>4.6229019265199801E-3</v>
+      </c>
+      <c r="N12" s="10">
+        <v>5.0319424126717199E-3</v>
+      </c>
+      <c r="O12" s="10">
+        <v>5.2589500430747097E-3</v>
+      </c>
+      <c r="P12" s="10">
+        <v>5.3707955131846504E-3</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>5.1974780209037702E-3</v>
+      </c>
+      <c r="R12" s="10">
+        <v>5.2858721555145904E-3</v>
+      </c>
+      <c r="S12" s="10">
+        <v>5.0925217503490104E-3</v>
+      </c>
+      <c r="T12" s="10">
+        <v>5.0645719354046898E-3</v>
+      </c>
+      <c r="U12" s="10">
+        <v>5.0696153700256303E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0.77725999999999995</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.36868000000000001</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.32253999999999999</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.29565000000000002</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.27445999999999998</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.25613000000000002</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.23913000000000001</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.22388</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.21010999999999999</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0.1978</v>
+      </c>
+      <c r="L13" s="10">
+        <v>1.15828609016368E-2</v>
+      </c>
+      <c r="M13" s="10">
+        <v>1.6226179121681401E-3</v>
+      </c>
+      <c r="N13" s="10">
+        <v>2.60563491942622E-3</v>
+      </c>
+      <c r="O13" s="10">
+        <v>3.2132538026119102E-3</v>
+      </c>
+      <c r="P13" s="10">
+        <v>3.8378813599866902E-3</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>4.1109744722037699E-3</v>
+      </c>
+      <c r="R13" s="10">
+        <v>4.2838326557210604E-3</v>
+      </c>
+      <c r="S13" s="10">
+        <v>4.2165810267983097E-3</v>
+      </c>
+      <c r="T13" s="10">
+        <v>3.9458698519957399E-3</v>
+      </c>
+      <c r="U13" s="10">
+        <v>3.7458124767680398E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0.77725999999999995</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.36867</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.32255</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.29565000000000002</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.27445999999999998</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.25613999999999998</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.23913999999999999</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.22388</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0.21012</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0.19780999999999899</v>
+      </c>
+      <c r="L14" s="10">
+        <v>1.15828609016368E-2</v>
+      </c>
+      <c r="M14" s="10">
+        <v>1.6337074401495499E-3</v>
+      </c>
+      <c r="N14" s="10">
+        <v>2.5846770698784698E-3</v>
+      </c>
+      <c r="O14" s="10">
+        <v>3.19869765164927E-3</v>
+      </c>
+      <c r="P14" s="10">
+        <v>3.8204711751300899E-3</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>4.0925949388295503E-3</v>
+      </c>
+      <c r="R14" s="10">
+        <v>4.2937163390237999E-3</v>
+      </c>
+      <c r="S14" s="10">
+        <v>4.2073480694824498E-3</v>
+      </c>
+      <c r="T14" s="10">
+        <v>3.91997732419745E-3</v>
+      </c>
+      <c r="U14" s="10">
+        <v>3.7400089126453499E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.61075999999999997</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.34963</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.33045999999999998</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.31795999999999902</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.31395999999999902</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.30613999999999902</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0.30691999999999903</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.30691000000000002</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.30409000000000003</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0.30719999999999997</v>
+      </c>
+      <c r="L15" s="10">
+        <v>1.8857724618250599E-2</v>
+      </c>
+      <c r="M15" s="10">
+        <v>5.97049225590134E-3</v>
+      </c>
+      <c r="N15" s="10">
+        <v>6.90011272049633E-3</v>
+      </c>
+      <c r="O15" s="10">
+        <v>3.85002164496078E-3</v>
+      </c>
+      <c r="P15" s="10">
+        <v>7.0882061670542998E-3</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>6.1204938072384699E-3</v>
+      </c>
+      <c r="R15" s="10">
+        <v>5.0481679845266504E-3</v>
+      </c>
+      <c r="S15" s="10">
+        <v>5.6433736954650199E-3</v>
+      </c>
+      <c r="T15" s="10">
+        <v>4.9688921188619697E-3</v>
+      </c>
+      <c r="U15" s="10">
+        <v>9.0730369777709801E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0.61538000000000004</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.35682000000000003</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.33335999999999999</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.32597999999999999</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.32099</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.32002000000000003</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.31941000000000003</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.32144</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.32368000000000002</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0.31931999999999999</v>
+      </c>
+      <c r="L16" s="10">
+        <v>2.2893123664347498E-2</v>
+      </c>
+      <c r="M16" s="10">
+        <v>8.2114824754391594E-3</v>
+      </c>
+      <c r="N16" s="10">
+        <v>6.17273575221445E-3</v>
+      </c>
+      <c r="O16" s="10">
+        <v>6.9568191965389903E-3</v>
+      </c>
+      <c r="P16" s="10">
+        <v>9.9791393527809899E-3</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>1.07114476664506E-2</v>
+      </c>
+      <c r="R16" s="10">
+        <v>1.0470004775548001E-2</v>
+      </c>
+      <c r="S16" s="10">
+        <v>1.06306893264526E-2</v>
+      </c>
+      <c r="T16" s="10">
+        <v>1.1098828767036601E-2</v>
+      </c>
+      <c r="U16" s="10">
+        <v>1.2044436244359601E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U16">
+    <sortCondition ref="K2:K16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496D1A1F-012A-4917-AFE9-7B3AC93860EF}">
   <dimension ref="A1:W223"/>
   <sheetViews>
@@ -13797,7 +14926,7 @@
     <col min="3" max="16" width="11.46484375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="57">
+    <row r="1" spans="1:23" ht="71.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>

</xml_diff>